<commit_message>
research smx dp added
</commit_message>
<xml_diff>
--- a/Engage/K12-Performance/src/main/resources/excelfiles/K12_Performance.xlsx
+++ b/Engage/K12-Performance/src/main/resources/excelfiles/K12_Performance.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
   <si>
     <t>Environment</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>8.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User Name not present on page.</t>
   </si>
 </sst>
 </file>
@@ -270,7 +273,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,8 +411,30 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="56">
+  <fills count="68">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +465,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -742,7 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -790,6 +875,14 @@
     <xf numFmtId="0" fontId="22" fillId="53" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="22" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="57" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="59" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="61" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="63" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="65" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="67" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1313,13 +1406,15 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="14" t="s">
-        <v>40</v>
+      <c r="J2" s="52" t="s">
+        <v>76</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="1"/>
       <c r="O2" s="4"/>

</xml_diff>